<commit_message>
add r script to generate baseline tables
</commit_message>
<xml_diff>
--- a/VSS Baseline.xlsx
+++ b/VSS Baseline.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://albanymedicalcenter-my.sharepoint.com/personal/sankarb_amc_edu/Documents/IIH Cosmos Study - Simha/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simhasankar/Documents/iih_medication_use_jns/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{C16951A6-3817-3F4D-BA38-627F32F2C64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB835339-3D73-D44E-A657-63310D26380C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65557B12-0A21-4C4E-8D99-83504E45A0B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29020" yWindow="820" windowWidth="20540" windowHeight="25560" xr2:uid="{9B43F3FE-7D61-0F49-B803-863FFBBC5DDC}"/>
   </bookViews>
@@ -477,7 +477,7 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -534,7 +534,9 @@
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">

</xml_diff>